<commit_message>
change "leung" to "leng"
</commit_message>
<xml_diff>
--- a/raw-data/GeneSets/README & Exemplar heatmap.xlsx
+++ b/raw-data/GeneSets/README & Exemplar heatmap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghokwon/Desktop/Lab/RNAseq dataset_VIFAD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sparthib/Documents/Visium_SPG_AD/raw-data/GeneSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E40D943-D1B1-4F45-8C26-B27367BD2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1BF7E-71EC-2543-98A8-880E927693D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="33600" windowHeight="18020" xr2:uid="{F6466BD4-5097-6544-AB98-7380CC9D7185}"/>
+    <workbookView xWindow="2140" yWindow="880" windowWidth="30240" windowHeight="18020" xr2:uid="{F6466BD4-5097-6544-AB98-7380CC9D7185}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="134">
   <si>
     <t>No pathology</t>
   </si>
@@ -1010,6 +1010,9 @@
   </si>
   <si>
     <t>OPC</t>
+  </si>
+  <si>
+    <t>Leng et al</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1449,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1478,18 +1481,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1511,113 +1505,122 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1625,16 +1628,34 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1645,66 +1666,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2030,22 +1991,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8AD549D-411D-2449-AED8-0803F3A24492}">
   <dimension ref="A1:I48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11:H13"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="101" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="12"/>
-    <col min="4" max="4" width="15" style="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.83203125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="108.5" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="187.1640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="12"/>
+    <col min="1" max="1" width="24" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="11"/>
+    <col min="4" max="4" width="15" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="108.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="187.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -2073,659 +2034,659 @@
       <c r="H1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="12" t="s">
+      <c r="I1" s="11" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="13">
+      <c r="C2" s="50">
         <v>2018</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="22"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="22" t="s">
+      <c r="A3" s="50"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="22" t="s">
+      <c r="A4" s="50"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="50"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="13" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="22" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="13" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="50" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="50">
         <v>2018</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="84" t="s">
+      <c r="H6" s="48" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="22" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="50"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="13" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="22" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="50"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="22" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="50"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="22" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="13" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="22" t="s">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="13" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="22" t="s">
+      <c r="A12" s="50"/>
+      <c r="B12" s="50"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="13" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="22" t="s">
+      <c r="A13" s="50"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="13" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="50">
         <v>2019</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="55" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="15" t="s">
+      <c r="A15" s="50"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="16"/>
+      <c r="H15" s="55"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="15" t="s">
+      <c r="A16" s="50"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="50"/>
+      <c r="E16" s="50"/>
+      <c r="F16" s="50"/>
+      <c r="G16" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="H16" s="16"/>
+      <c r="H16" s="55"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="15" t="s">
+      <c r="A17" s="50"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="50"/>
+      <c r="E17" s="50"/>
+      <c r="F17" s="50"/>
+      <c r="G17" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="16"/>
+      <c r="H17" s="55"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="17" t="s">
+      <c r="A18" s="50"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="50"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H18" s="16" t="s">
+      <c r="H18" s="55" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" s="13"/>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="17" t="s">
+      <c r="A19" s="50"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="50"/>
+      <c r="E19" s="50"/>
+      <c r="F19" s="50"/>
+      <c r="G19" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H19" s="16"/>
+      <c r="H19" s="55"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="17" t="s">
+      <c r="A20" s="50"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="50"/>
+      <c r="E20" s="50"/>
+      <c r="F20" s="50"/>
+      <c r="G20" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="H20" s="16"/>
+      <c r="H20" s="55"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="17" t="s">
+      <c r="A21" s="50"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="50"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
+      <c r="G21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="16"/>
+      <c r="H21" s="55"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-      <c r="E22" s="13"/>
-      <c r="F22" s="13"/>
-      <c r="G22" s="18" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="55" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="18" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="16"/>
+      <c r="H23" s="55"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" s="13"/>
-      <c r="B24" s="13"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
-      <c r="G24" s="18" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="50"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
+      <c r="G24" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H24" s="16"/>
+      <c r="H24" s="55"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="18" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="50"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="H25" s="16"/>
+      <c r="H25" s="55"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="19" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H26" s="55" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="19" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="50"/>
+      <c r="D27" s="50"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="16"/>
+      <c r="H27" s="55"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="19" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="50"/>
+      <c r="C28" s="50"/>
+      <c r="D28" s="50"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="H28" s="16"/>
+      <c r="H28" s="55"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="13"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-      <c r="G29" s="19" t="s">
+      <c r="A29" s="50"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="H29" s="16"/>
+      <c r="H29" s="55"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-      <c r="G30" s="20" t="s">
+      <c r="A30" s="50"/>
+      <c r="B30" s="50"/>
+      <c r="C30" s="50"/>
+      <c r="D30" s="50"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
+      <c r="G30" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="55" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="20" t="s">
+      <c r="A31" s="50"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="50"/>
+      <c r="D31" s="50"/>
+      <c r="E31" s="50"/>
+      <c r="F31" s="50"/>
+      <c r="G31" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="16"/>
+      <c r="H31" s="55"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="20" t="s">
+      <c r="A32" s="50"/>
+      <c r="B32" s="50"/>
+      <c r="C32" s="50"/>
+      <c r="D32" s="50"/>
+      <c r="E32" s="50"/>
+      <c r="F32" s="50"/>
+      <c r="G32" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="H32" s="16"/>
+      <c r="H32" s="55"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="13"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-      <c r="G33" s="20" t="s">
+      <c r="A33" s="50"/>
+      <c r="B33" s="50"/>
+      <c r="C33" s="50"/>
+      <c r="D33" s="50"/>
+      <c r="E33" s="50"/>
+      <c r="F33" s="50"/>
+      <c r="G33" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="H33" s="16"/>
+      <c r="H33" s="55"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="13"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-      <c r="G34" s="21" t="s">
+      <c r="A34" s="50"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="50"/>
+      <c r="D34" s="50"/>
+      <c r="E34" s="50"/>
+      <c r="F34" s="50"/>
+      <c r="G34" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="55" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="13"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-      <c r="G35" s="21" t="s">
+      <c r="A35" s="50"/>
+      <c r="B35" s="50"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="50"/>
+      <c r="E35" s="50"/>
+      <c r="F35" s="50"/>
+      <c r="G35" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="H35" s="16"/>
+      <c r="H35" s="55"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="13"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-      <c r="G36" s="21" t="s">
+      <c r="A36" s="50"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="50"/>
+      <c r="D36" s="50"/>
+      <c r="E36" s="50"/>
+      <c r="F36" s="50"/>
+      <c r="G36" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="H36" s="16"/>
+      <c r="H36" s="55"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="13"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="21" t="s">
+      <c r="A37" s="50"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="50"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="H37" s="16"/>
+      <c r="H37" s="55"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="50" t="s">
         <v>92</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="C38" s="13">
+      <c r="C38" s="50">
         <v>2019</v>
       </c>
-      <c r="D38" s="13" t="s">
+      <c r="D38" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="14" t="s">
+      <c r="F38" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="H38" s="22" t="s">
+      <c r="H38" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-      <c r="G39" s="22" t="s">
+      <c r="A39" s="50"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="50"/>
+      <c r="D39" s="50"/>
+      <c r="E39" s="50"/>
+      <c r="F39" s="50"/>
+      <c r="G39" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="13" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="13"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="22" t="s">
+      <c r="A40" s="50"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="50"/>
+      <c r="D40" s="50"/>
+      <c r="E40" s="50"/>
+      <c r="F40" s="50"/>
+      <c r="G40" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
-      <c r="C41" s="13"/>
-      <c r="D41" s="13"/>
-      <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="22" t="s">
+      <c r="A41" s="50"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="50"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H41" s="22" t="s">
+      <c r="H41" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="22" t="s">
+      <c r="A42" s="50"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="50"/>
+      <c r="D42" s="50"/>
+      <c r="E42" s="50"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="22" t="s">
+      <c r="A43" s="50"/>
+      <c r="B43" s="50"/>
+      <c r="C43" s="50"/>
+      <c r="D43" s="50"/>
+      <c r="E43" s="50"/>
+      <c r="F43" s="50"/>
+      <c r="G43" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="H43" s="22" t="s">
+      <c r="H43" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="13"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-      <c r="G44" s="22" t="s">
+      <c r="A44" s="50"/>
+      <c r="B44" s="50"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="F44" s="50"/>
+      <c r="G44" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H44" s="22" t="s">
+      <c r="H44" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="53" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C45" s="23">
+      <c r="B45" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="C45" s="53">
         <v>2021</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="F45" s="85" t="s">
+      <c r="F45" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="G45" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="13" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="24"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="24"/>
-      <c r="F46" s="86"/>
-      <c r="G46" s="22" t="s">
+      <c r="A46" s="54"/>
+      <c r="B46" s="54"/>
+      <c r="C46" s="54"/>
+      <c r="D46" s="54"/>
+      <c r="E46" s="54"/>
+      <c r="F46" s="52"/>
+      <c r="G46" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="13" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2733,25 +2694,25 @@
       <c r="A47" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B47" s="13" t="s">
+      <c r="B47" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="C47" s="13">
+      <c r="C47" s="50">
         <v>2021</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D47" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="F47" s="14" t="s">
+      <c r="F47" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G47" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="H47" s="22" t="s">
+      <c r="H47" s="13" t="s">
         <v>117</v>
       </c>
     </row>
@@ -2759,50 +2720,20 @@
       <c r="A48" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
-      <c r="F48" s="14"/>
-      <c r="G48" s="22" t="s">
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="50"/>
+      <c r="F48" s="49"/>
+      <c r="G48" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="H48" s="22" t="s">
+      <c r="H48" s="13" t="s">
         <v>121</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="F47:F48"/>
-    <mergeCell ref="E47:E48"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="E14:E37"/>
-    <mergeCell ref="E38:E44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="E6:E13"/>
-    <mergeCell ref="E2:E5"/>
-    <mergeCell ref="A38:A44"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="F14:F37"/>
-    <mergeCell ref="D14:D37"/>
-    <mergeCell ref="C14:C37"/>
-    <mergeCell ref="B14:B37"/>
-    <mergeCell ref="A14:A37"/>
-    <mergeCell ref="B38:B44"/>
-    <mergeCell ref="C38:C44"/>
-    <mergeCell ref="D38:D44"/>
-    <mergeCell ref="F38:F44"/>
-    <mergeCell ref="H14:H17"/>
-    <mergeCell ref="H18:H21"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="H26:H29"/>
-    <mergeCell ref="H30:H33"/>
     <mergeCell ref="H34:H37"/>
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="A2:A5"/>
@@ -2814,6 +2745,36 @@
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="F2:F5"/>
+    <mergeCell ref="H14:H17"/>
+    <mergeCell ref="H18:H21"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="H26:H29"/>
+    <mergeCell ref="H30:H33"/>
+    <mergeCell ref="E2:E5"/>
+    <mergeCell ref="A38:A44"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D14:D37"/>
+    <mergeCell ref="C14:C37"/>
+    <mergeCell ref="B14:B37"/>
+    <mergeCell ref="A14:A37"/>
+    <mergeCell ref="B38:B44"/>
+    <mergeCell ref="C38:C44"/>
+    <mergeCell ref="D38:D44"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="E14:E37"/>
+    <mergeCell ref="E38:E44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="E6:E13"/>
+    <mergeCell ref="F14:F37"/>
+    <mergeCell ref="F38:F44"/>
+    <mergeCell ref="F47:F48"/>
+    <mergeCell ref="E47:E48"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="B47:B48"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F2" r:id="rId1" xr:uid="{E9832EC8-1720-B14B-8F14-4013C54BA34F}"/>
@@ -2843,29 +2804,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="65" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="67"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
     </row>
     <row r="2" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
@@ -2876,18 +2837,18 @@
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="7"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
     </row>
     <row r="3" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="4" t="s">
@@ -2897,19 +2858,19 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="12"/>
-      <c r="S3" s="12"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
     </row>
     <row r="4" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="4" t="s">
@@ -2919,19 +2880,19 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="12"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="11"/>
     </row>
     <row r="5" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4" t="s">
@@ -2941,41 +2902,41 @@
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="11"/>
     </row>
     <row r="6" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="75"/>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="76"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="12"/>
-      <c r="R6" s="12"/>
-      <c r="S6" s="12"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
+      <c r="R6" s="11"/>
+      <c r="S6" s="11"/>
     </row>
     <row r="7" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="4" t="s">
@@ -2985,19 +2946,19 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="Q7" s="11"/>
+      <c r="R7" s="11"/>
+      <c r="S7" s="11"/>
     </row>
     <row r="8" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
@@ -3007,19 +2968,19 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="12"/>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="12"/>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="Q8" s="11"/>
+      <c r="R8" s="11"/>
+      <c r="S8" s="11"/>
     </row>
     <row r="9" spans="2:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
@@ -3037,362 +2998,362 @@
       <c r="F9" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="12"/>
-      <c r="I9" s="12"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="12"/>
-      <c r="Q9" s="12"/>
-      <c r="R9" s="12"/>
-      <c r="S9" s="12"/>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="Q9" s="11"/>
+      <c r="R9" s="11"/>
+      <c r="S9" s="11"/>
     </row>
     <row r="10" spans="2:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="34" t="s">
+      <c r="C10" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="12"/>
-      <c r="Q10" s="12"/>
-      <c r="R10" s="12"/>
-      <c r="S10" s="12"/>
-      <c r="T10" s="12"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
     </row>
     <row r="11" spans="2:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="25"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
       <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="12"/>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="12"/>
-      <c r="S11" s="12"/>
-      <c r="T11" s="12"/>
-      <c r="U11" s="12"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11"/>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
+      <c r="U11" s="11"/>
     </row>
     <row r="12" spans="2:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="35" t="s">
+      <c r="B12" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="60" t="s">
         <v>92</v>
       </c>
-      <c r="D12" s="68"/>
-      <c r="E12" s="68"/>
-      <c r="F12" s="68"/>
-      <c r="G12" s="68"/>
-      <c r="H12" s="68"/>
-      <c r="I12" s="68"/>
-      <c r="J12" s="68"/>
-      <c r="K12" s="68"/>
-      <c r="L12" s="68"/>
-      <c r="M12" s="68"/>
-      <c r="N12" s="68"/>
-      <c r="O12" s="68"/>
-      <c r="P12" s="68"/>
-      <c r="Q12" s="68"/>
-      <c r="R12" s="68"/>
-      <c r="S12" s="68"/>
-      <c r="T12" s="68"/>
-      <c r="U12" s="68"/>
-      <c r="V12" s="69"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="61"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+      <c r="L12" s="61"/>
+      <c r="M12" s="61"/>
+      <c r="N12" s="61"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="61"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="61"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="61"/>
+      <c r="U12" s="61"/>
+      <c r="V12" s="62"/>
     </row>
     <row r="13" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="39"/>
-      <c r="E13" s="39"/>
-      <c r="F13" s="39"/>
-      <c r="G13" s="39"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="60"/>
-      <c r="L13" s="51"/>
-      <c r="M13" s="51"/>
-      <c r="N13" s="51"/>
-      <c r="O13" s="48"/>
-      <c r="P13" s="48"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="51"/>
-      <c r="S13" s="51"/>
-      <c r="T13" s="51"/>
-      <c r="U13" s="51"/>
-      <c r="V13" s="52"/>
+      <c r="C13" s="25"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="42"/>
+      <c r="J13" s="42"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="35"/>
+      <c r="M13" s="35"/>
+      <c r="N13" s="35"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="35"/>
+      <c r="S13" s="35"/>
+      <c r="T13" s="35"/>
+      <c r="U13" s="35"/>
+      <c r="V13" s="36"/>
     </row>
     <row r="14" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="40"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="41"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="53"/>
-      <c r="N14" s="53"/>
-      <c r="O14" s="49"/>
-      <c r="P14" s="49"/>
-      <c r="Q14" s="53"/>
-      <c r="R14" s="53"/>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="53"/>
-      <c r="V14" s="54"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="37"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="38"/>
     </row>
     <row r="15" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="40"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
-      <c r="H15" s="41"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="53"/>
-      <c r="N15" s="53"/>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="53"/>
-      <c r="R15" s="53"/>
-      <c r="S15" s="53"/>
-      <c r="T15" s="53"/>
-      <c r="U15" s="53"/>
-      <c r="V15" s="54"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
+      <c r="N15" s="37"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="37"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="38"/>
     </row>
     <row r="16" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C16" s="40"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="53"/>
-      <c r="M16" s="53"/>
-      <c r="N16" s="53"/>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="53"/>
-      <c r="S16" s="53"/>
-      <c r="T16" s="53"/>
-      <c r="U16" s="53"/>
-      <c r="V16" s="54"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="37"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="37"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="37"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="37"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="38"/>
     </row>
     <row r="17" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="74" t="s">
+      <c r="B17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="40"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
-      <c r="G17" s="41"/>
-      <c r="H17" s="41"/>
-      <c r="I17" s="61"/>
-      <c r="J17" s="61"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="53"/>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
-      <c r="Q17" s="53"/>
-      <c r="R17" s="53"/>
-      <c r="S17" s="53"/>
-      <c r="T17" s="53"/>
-      <c r="U17" s="53"/>
-      <c r="V17" s="54"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="37"/>
+      <c r="M17" s="37"/>
+      <c r="N17" s="37"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="37"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="37"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="38"/>
     </row>
     <row r="18" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="40"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="41"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="61"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="49"/>
-      <c r="P18" s="49"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="54"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="37"/>
+      <c r="N18" s="37"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="37"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="37"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="38"/>
     </row>
     <row r="19" spans="2:22" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="40"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="61"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="49"/>
-      <c r="P19" s="49"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="54"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="37"/>
+      <c r="M19" s="37"/>
+      <c r="N19" s="37"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="37"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="37"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="38"/>
     </row>
     <row r="20" spans="2:22" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="42" t="s">
+      <c r="C20" s="29" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="43" t="s">
+      <c r="D20" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="43" t="s">
+      <c r="F20" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="G20" s="44" t="s">
+      <c r="G20" s="31" t="s">
         <v>131</v>
       </c>
-      <c r="H20" s="45" t="s">
+      <c r="H20" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="I20" s="55" t="s">
+      <c r="I20" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="55" t="s">
+      <c r="J20" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="K20" s="55" t="s">
+      <c r="K20" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="L20" s="55" t="s">
+      <c r="L20" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="M20" s="56" t="s">
+      <c r="M20" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="N20" s="62" t="s">
+      <c r="N20" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="O20" s="50" t="s">
+      <c r="O20" s="34" t="s">
         <v>126</v>
       </c>
-      <c r="P20" s="50" t="s">
+      <c r="P20" s="34" t="s">
         <v>123</v>
       </c>
-      <c r="Q20" s="55" t="s">
+      <c r="Q20" s="39" t="s">
         <v>122</v>
       </c>
-      <c r="R20" s="55" t="s">
+      <c r="R20" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="S20" s="55" t="s">
+      <c r="S20" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="T20" s="55" t="s">
+      <c r="T20" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="U20" s="56" t="s">
+      <c r="U20" s="40" t="s">
         <v>131</v>
       </c>
-      <c r="V20" s="57" t="s">
+      <c r="V20" s="41" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="21" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="36" t="s">
+      <c r="B21" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="46" t="s">
+      <c r="C21" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="D21" s="47"/>
-      <c r="E21" s="47"/>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="63" t="s">
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="56" t="s">
         <v>13</v>
       </c>
-      <c r="J21" s="63"/>
-      <c r="K21" s="63"/>
-      <c r="L21" s="63"/>
-      <c r="M21" s="63"/>
-      <c r="N21" s="63"/>
-      <c r="O21" s="47" t="s">
+      <c r="J21" s="56"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="56"/>
+      <c r="M21" s="56"/>
+      <c r="N21" s="56"/>
+      <c r="O21" s="57" t="s">
         <v>15</v>
       </c>
-      <c r="P21" s="47"/>
+      <c r="P21" s="57"/>
       <c r="Q21" s="58" t="s">
         <v>16</v>
       </c>
@@ -3404,142 +3365,142 @@
     </row>
     <row r="22" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="64" t="s">
+      <c r="C23" s="70" t="s">
         <v>128</v>
       </c>
-      <c r="D23" s="65"/>
-      <c r="E23" s="65"/>
-      <c r="F23" s="65"/>
-      <c r="G23" s="65"/>
-      <c r="H23" s="66"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="72"/>
     </row>
     <row r="24" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72"/>
-      <c r="H24" s="73"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="75"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="76"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="20"/>
     </row>
     <row r="26" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="75"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="76"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="20"/>
     </row>
     <row r="27" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="75"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="76"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="20"/>
     </row>
     <row r="28" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="75"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="76"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="20"/>
     </row>
     <row r="29" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="75"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="76"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="20"/>
     </row>
     <row r="30" spans="2:22" x14ac:dyDescent="0.2">
-      <c r="B30" s="74" t="s">
+      <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="75"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="76"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="2:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="77" t="s">
+      <c r="C31" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="D31" s="78" t="s">
+      <c r="D31" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="78" t="s">
+      <c r="E31" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="F31" s="78" t="s">
+      <c r="F31" s="45" t="s">
         <v>125</v>
       </c>
-      <c r="G31" s="79" t="s">
+      <c r="G31" s="46" t="s">
         <v>131</v>
       </c>
-      <c r="H31" s="80" t="s">
+      <c r="H31" s="47" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" spans="2:22" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="36" t="s">
+      <c r="B32" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C32" s="81" t="s">
+      <c r="C32" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="82"/>
-      <c r="E32" s="82"/>
-      <c r="F32" s="82"/>
-      <c r="G32" s="82"/>
-      <c r="H32" s="83"/>
+      <c r="D32" s="63"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="63"/>
+      <c r="G32" s="63"/>
+      <c r="H32" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C21:H21"/>
+    <mergeCell ref="C32:H32"/>
+    <mergeCell ref="C23:H23"/>
     <mergeCell ref="I21:N21"/>
     <mergeCell ref="O21:P21"/>
     <mergeCell ref="Q21:V21"/>
     <mergeCell ref="C12:V12"/>
     <mergeCell ref="D10:G10"/>
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="C21:H21"/>
-    <mergeCell ref="C32:H32"/>
-    <mergeCell ref="C23:H23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>